<commit_message>
Resolved merge conflicts and updated pending request logic
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="59">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,139 +43,151 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-27T06:05:59.685Z</t>
+    <t>2025-11-27T08:58:44.660Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bf84f8f2-3f54-4a65-a3d7-8cadc58d16ad","EventDtm":"2025-11-27T05:38:02Z","AppDtm":"2025-11-27T05:38:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:38:02Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.657927,"GPSLongitude":83.101635,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8.1,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:38:02Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":31.63,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":67.36,"PSucQ":null,"TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":124.8,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.91,"AmpPhB":1.54,"AmpPhC":0.91,"PDis":125.35,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.47,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.06,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.4,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.22,"TRtn1Q":null,"TRtn2":20.28,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":17.05,"PctSucVlvQ":null,"TSup1":18.61,"TSup1Q":null,"TSup2":18.71,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.760Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fa3e844d-49af-4de2-9793-56db683115a8","EventDtm":"2025-11-27T05:38:31Z","AppDtm":"2025-11-27T05:38:45Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:38:31Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.606219,"GPSLongitude":80.723448,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.763Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4ecb69eb-156a-4c5b-a9ea-ca681982d8d1","EventDtm":"2025-11-27T05:38:37Z","AppDtm":"2025-11-27T05:38:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:38:37Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892132,"GPSLongitude":79.476239,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:38:37Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":28.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":77.7,"TDisQ":null,"FreqComp":null,"TSuc":-25.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":850,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":21,"PctExpVlvQ":null,"TEvap":-1.69,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":396.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.38,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.89,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.785Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"770befe9-c826-4294-a65e-cd2aea7da655","EventDtm":"2025-11-27T05:39:27Z","AppDtm":"2025-11-27T05:39:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:39:27Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.572376,"GPSLongitude":78.515054,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"230807317","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":33.5,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.787Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f2e4bfb-b93f-43b5-a8a4-bac53880e157","EventDtm":"2025-11-27T05:41:49Z","AppDtm":"2025-11-27T05:42:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:41:49Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.658002,"GPSLongitude":83.101741,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":7.9,"DeviceTemp":50,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:41:49Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":32.2,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":61.77,"PSucQ":null,"TDis":-188.28,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":139.98,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.92,"AmpPhB":1.54,"AmpPhC":0.92,"PDis":154.15,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.61,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.99,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.33,"TRtn1Q":null,"TRtn2":20.35,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":16.62,"PctSucVlvQ":null,"TSup1":19.6,"TSup1Q":null,"TSup2":19.65,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.814Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0e2bdd47-f96e-44ae-b804-8fc56c217372","EventDtm":"2025-11-27T05:42:16Z","AppDtm":"2025-11-27T05:42:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:42:16Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":16.892152,"GPSLongitude":79.476162,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-61","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:42:16Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":30.41,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":138.03,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":11.2,"AmpPhB":10.92,"AmpPhC":11.2,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.17,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.21,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":402.8,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.88,"TRtn1Q":null,"TRtn2":17.83,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.19,"PctSucVlvQ":null,"TSup1":18.56,"TSup1Q":null,"TSup2":18.59,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.830Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"314440c1-7eb2-4663-94a3-16306eb4a0a2","EventDtm":"2025-11-27T05:42:34Z","AppDtm":"2025-11-27T05:42:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:42:34Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":12.805053,"GPSLongitude":77.662169,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:42:34Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":24.1,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":96.49,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":11.01,"AmpPhB":10.53,"AmpPhC":11.01,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.98,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.33,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.42,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.33,"TRtn1Q":null,"TRtn2":5.34,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":2.8,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.835Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"cec3478b-dc7c-4d0b-8693-ea9a61f515d3","EventDtm":"2025-11-27T05:44:50Z","AppDtm":"2025-11-27T05:45:07Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:44:50Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.804944,"GPSLongitude":77.66222,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:44:50Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.55,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":94.55,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.37,"AmpPhB":10.77,"AmpPhC":11.37,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.13,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.93,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.71,"TRtn1Q":null,"TRtn2":5.73,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.51,"PctSucVlvQ":null,"TSup1":5.04,"TSup1Q":null,"TSup2":5.2,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.837Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7d3563fd-9e72-438b-8d19-7a15fe03435b","EventDtm":"2025-11-27T05:54:51Z","AppDtm":"2025-11-27T05:55:07Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:54:51Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.804959,"GPSLongitude":77.662203,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:54:51Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.73,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":97.68,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.43,"AmpPhB":11.01,"AmpPhC":11.43,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.64,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.05,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.78,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.16,"PctSucVlvQ":null,"TSup1":5.05,"TSup1Q":null,"TSup2":5.21,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.838Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"132dc001-7507-4fe2-9d13-6f969a8ca657","EventDtm":"2025-11-27T07:38:38Z","AppDtm":"2025-11-27T05:56:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T07:38:38Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":6627,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":34.2,"BatteryVoltage":8.1,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.854Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b43874a7-6d12-4f37-94ba-ded471b6f0c9","EventDtm":"2025-11-27T05:59:17Z","AppDtm":"2025-11-27T05:59:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T05:59:17Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.539093,"GPSLongitude":78.178293,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T05:59:17Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":29.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":101.3,"TDisQ":null,"FreqComp":null,"TSuc":-32,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":930,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":411,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":90.55,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.866Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bb2737f9-9664-4b84-8155-9330b263efa7","EventDtm":"2025-11-27T06:00:05Z","AppDtm":"2025-11-27T06:00:22Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:00:05Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.310563,"GPSLongitude":91.717529,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":false,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.869Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"98423f22-4d59-4c54-b7c4-e4d0b1a46a03","EventDtm":"2025-11-27T06:00:06Z","AppDtm":"2025-11-27T06:00:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:00:06Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533113,"GPSLongitude":78.433442,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:00:06Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":28,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":76.5,"TDisQ":null,"FreqComp":null,"TSuc":-29.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":414.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6,"TRtn1Q":null,"TRtn2":6.1,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.871Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"64a53b7c-0200-4268-a8e1-d515f47af216","EventDtm":"2025-11-27T06:01:18Z","AppDtm":"2025-11-27T06:01:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:01:18Z","DeviceID":"JSGA623040321","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":12.81637,"GPSLongitude":77.687293,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"7055","CID":"103377676","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6617250","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.877Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b98ed436-278e-4d1a-9481-0ae6e9a5be47","EventDtm":"2025-11-27T06:01:39Z","AppDtm":"2025-11-27T06:01:55Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:01:39Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.310576,"GPSLongitude":91.717536,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.4,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:01:39Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":28.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":58.8,"TDisQ":null,"FreqComp":null,"TSuc":2,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":230,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":35,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":411,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":44.88,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":46.04,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.882Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fae2366f-f885-4139-bd93-682aa8e12ff9","EventDtm":"2025-11-27T06:04:24Z","AppDtm":"2025-11-27T06:04:39Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:04:24Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.310567,"GPSLongitude":91.717565,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.1,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:04:24Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":29.19,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":250,"PSucQ":"asProvided","TDis":53.4,"TDisQ":null,"FreqComp":null,"TSuc":4.6,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":240,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":50,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"PTIEmergencyStop1","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":403,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":45.19,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":46.65,"PctSucVlvQ":null,"TSup1":5.38,"TSup1Q":null,"TSup2":5.2,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.884Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"cf032045-1028-42dc-bd04-c64cac2cd2c1","EventDtm":"2025-11-27T06:04:44Z","AppDtm":"2025-11-27T06:04:58Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:04:44Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.644569,"GPSLongitude":88.468022,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323862","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8.1,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:04:44Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":29,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":68.8,"TDisQ":null,"FreqComp":null,"TSuc":-21.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1020,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":29,"PctExpVlvQ":null,"TEvap":-1.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":408.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":1.38,"TRtn1Q":null,"TRtn2":2.1,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":14.02,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.887Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30da834f-17ec-4e53-87b6-5bf348ada453","EventDtm":"2025-11-27T06:04:54Z","AppDtm":"2025-11-27T06:05:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:04:54Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.804997,"GPSLongitude":77.662173,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:04:54Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.41,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":94.89,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.61,"AmpPhB":11.03,"AmpPhC":11.61,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.22,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.72,"TRtn1Q":null,"TRtn2":5.74,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.41,"PctSucVlvQ":null,"TSup1":4.91,"TSup1Q":null,"TSup2":5.07,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.890Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"de73508a-dd45-430c-aada-c4ee15843ec0","EventDtm":"2025-11-27T06:05:04Z","AppDtm":"2025-11-27T06:05:17Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:05:04Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.606171,"GPSLongitude":80.723575,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":7.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:05:59.894Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6b0b845f-9aa9-412b-b84d-9483cc904c45","EventDtm":"2025-11-27T06:05:30Z","AppDtm":"2025-11-27T06:05:47Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:05:30Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.310572,"GPSLongitude":91.717576,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.3,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:05:30Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":29.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":170,"PSucQ":"asProvided","TDis":51.5,"TDisQ":null,"FreqComp":null,"TSuc":4.1,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1360,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":100,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":403,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.9,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":115.24,"PctSucVlvQ":null,"TSup1":5.62,"TSup1Q":null,"TSup2":5.4,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:08:33.756Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c14785fa-5292-4626-900b-2c4137af0739","EventDtm":"2025-11-27T06:08:15Z","AppDtm":"2025-11-27T06:08:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:08:15Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":16.824925,"GPSLongitude":78.13147,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":46,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:08:15Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":32.38,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":75.8,"TDisQ":null,"FreqComp":null,"TSuc":-23.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1110,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":394.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.28,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T06:10:38.359Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1b270b95-de63-49fa-80fb-d52d88854732","EventDtm":"2025-11-27T06:10:21Z","AppDtm":"2025-11-27T06:10:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T06:10:21Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.661649,"GPSLongitude":83.089113,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T06:10:21Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.19,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":46.4,"TDisQ":null,"FreqComp":null,"TSuc":-13.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1070,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":368.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":99.09,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7ae7e736-a46c-41ba-b21b-2124282916a3","EventDtm":"2025-11-27T08:19:55Z","AppDtm":"2025-11-27T08:20:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:19:55Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":15.479492,"GPSLongitude":73.969788,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":28.7,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:19:55Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.58,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.62,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.43,"AmpPhB":9.86,"AmpPhC":10.43,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.01,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.22,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.63,"TRtn1Q":null,"TRtn2":5.65,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.38,"PctSucVlvQ":null,"TSup1":5.03,"TSup1Q":null,"TSup2":5.05,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.714Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8a387fa6-01ab-4e94-8748-62a1e5febbeb","EventDtm":"2025-11-27T08:20:42Z","AppDtm":"2025-11-27T08:20:58Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:20:42Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":26.310538,"GPSLongitude":91.717547,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":46,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:20:42Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":32.69,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":83.7,"TDisQ":null,"FreqComp":null,"TSuc":-22.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1090,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":73,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":397.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":100.61,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.746Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2ddc8839-f45e-46bc-8d8b-969c463245ca","EventDtm":"2025-11-27T08:22:47Z","AppDtm":"2025-11-27T08:23:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:22:47Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.533509,"GPSLongitude":78.433139,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:22:47Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":29.19,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":66,"TDisQ":null,"FreqComp":null,"TSuc":19.4,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":930,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.17,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":422.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.5,"TRtn1Q":null,"TRtn2":135.9,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":90.24,"PctSucVlvQ":null,"TSup1":4.38,"TSup1Q":null,"TSup2":4.5,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.760Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1a277cd7-e85a-46de-854c-7cfa88c989ee","EventDtm":"2025-11-27T08:23:19Z","AppDtm":"2025-11-27T08:23:39Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:23:19Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.516029,"GPSLongitude":82.981279,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:23:19Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":29.23,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.48,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":132.09,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.43,"AmpPhB":10.86,"AmpPhC":11.43,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.12,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.75,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.74,"TRtn1Q":null,"TRtn2":3.78,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.41,"PctSucVlvQ":null,"TSup1":3,"TSup1Q":null,"TSup2":3.06,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.776Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"13fbbc28-651f-45af-b2db-7dd46d6b6a34","EventDtm":"2025-11-27T08:24:25Z","AppDtm":"2025-11-27T08:24:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:24:25Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.547798,"GPSLongitude":78.380557,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.7,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.846Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"40359c31-6e8c-4a06-b6b9-d80191a96856","EventDtm":"2025-11-27T08:24:58Z","AppDtm":"2025-11-27T08:25:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:24:58Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804904,"GPSLongitude":77.662287,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:24:58Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.99,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":96.16,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.74,"AmpPhB":11.15,"AmpPhC":11.74,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.23,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.07,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.81,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.83,"PctSucVlvQ":null,"TSup1":5.02,"TSup1Q":null,"TSup2":4.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.858Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"cde8c4fd-d49d-426b-b49b-46f7124980eb","EventDtm":"2025-11-27T08:25:39Z","AppDtm":"2025-11-27T08:26:00Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:25:39Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":21.735681,"GPSLongitude":72.628731,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"236857089","RSSI":"-61","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:25:39Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":37.2,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":228.51,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":14.19,"AmpPhB":13.94,"AmpPhC":14.19,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.46,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89.61,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":434.83,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.74,"TRtn1Q":null,"TRtn2":15.69,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.65,"PctSucVlvQ":null,"TSup1":15,"TSup1Q":null,"TSup2":15.18,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.875Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b50aa7a9-e373-4eb4-81de-9fb35a9ba547","EventDtm":"2025-11-27T08:27:00Z","AppDtm":"2025-11-27T08:27:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:27:00Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.516174,"GPSLongitude":82.962357,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:27:00Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":28.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":82,"TDisQ":null,"FreqComp":null,"TSuc":-11.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":52,"PctExpVlvQ":null,"TEvap":22.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":380.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.7,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.2,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.881Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"77460620-84e2-4659-8eca-ed12d417f019","EventDtm":"2025-11-27T08:29:31Z","AppDtm":"2025-11-27T08:29:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:29:31Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":4,"GPSLatitude":19.252837,"GPSLongitude":73.01647,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.894Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6c3abb16-7eb2-4453-81bb-a38cec717503","EventDtm":"2025-11-27T08:32:48Z","AppDtm":"2025-11-27T08:33:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:32:48Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":16.891824,"GPSLongitude":79.47598,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:32:48Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":30.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":73.7,"TDisQ":null,"FreqComp":null,"TSuc":-29.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":960,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":401.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.62,"TRtn1Q":null,"TRtn2":36.7,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.902Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c02b4cf7-7a3b-40e0-92e9-a94d4931d1e5","EventDtm":"2025-11-27T08:34:54Z","AppDtm":"2025-11-27T08:35:10Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:34:54Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804909,"GPSLongitude":77.662315,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:34:54Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.94,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":96.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.62,"AmpPhB":11.02,"AmpPhC":11.62,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.99,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.05,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.82,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.78,"PctSucVlvQ":null,"TSup1":5.05,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.908Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"86890180-2fd2-4e8e-866c-d84c0c8cde93","EventDtm":"2025-11-27T08:37:24Z","AppDtm":"2025-11-27T08:37:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:37:24Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.657855,"GPSLongitude":83.101833,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.5,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:37:24Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":29.99,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":72.12,"PSucQ":null,"TDis":-190.23,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":111.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.94,"AmpPhB":1.56,"AmpPhC":0.94,"PDis":111.37,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.3,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.03,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":425.64,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.95,"TRtn1Q":null,"TRtn2":21,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":18.37,"PctSucVlvQ":null,"TSup1":21.24,"TSup1Q":null,"TSup2":21.32,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.912Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bffab387-2a02-4c5c-94da-81386159f700","EventDtm":"2025-11-27T08:31:21Z","AppDtm":"2025-11-27T08:38:21Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:31:21Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":28.364638,"GPSLongitude":75.581309,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-83","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:31:21Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":22,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":35,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":6,"AmpPhB":6.8,"AmpPhC":6.8,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.3,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":6.4,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.918Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d312fbd9-7f70-428d-a4f2-6108c28531f2","EventDtm":"2025-11-27T08:38:18Z","AppDtm":"2025-11-27T08:38:39Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:38:18Z","DeviceID":"JSGA623040314","GPSLockState":"UNLOCKED","GPSSatelliteCount":11,"GPSLastLock":8,"GPSLatitude":19.252914,"GPSLongitude":73.01652,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:38:18Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":25.4,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":144.31,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":11.33,"AmpPhB":11.68,"AmpPhC":11.33,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.83,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.99,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.11,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.32,"TRtn1Q":null,"TRtn2":5.45,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":3.21,"PctSucVlvQ":null,"TSup1":8.03,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.925Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"066224c0-21eb-4e5c-a74f-330cdd40144c","EventDtm":"2025-11-27T08:38:40Z","AppDtm":"2025-11-27T08:38:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:38:40Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":16.892067,"GPSLongitude":79.476275,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.3,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:38:40Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":30.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":82.6,"TDisQ":null,"FreqComp":null,"TSuc":-26.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":920,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":21,"PctExpVlvQ":null,"TEvap":-1.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":399.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.69,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.5,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.928Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"92b41552-47db-4444-9076-3a456be9e7ef","EventDtm":"2025-11-27T08:39:01Z","AppDtm":"2025-11-27T08:39:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:39:01Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":9,"GPSLastLock":232,"GPSLatitude":17.547993,"GPSLongitude":78.380501,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.930Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8f9d67d0-c0fa-479c-ae2d-c92825325fae","EventDtm":"2025-11-27T08:39:37Z","AppDtm":"2025-11-27T08:39:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:39:37Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":26.606059,"GPSLongitude":80.723835,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":41,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.931Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c9118033-f00b-499c-b09f-10090e9510b6","EventDtm":"2025-11-27T08:42:20Z","AppDtm":"2025-11-27T08:42:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:42:20Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.657886,"GPSLongitude":83.101752,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.4,"BatteryVoltage":7.9,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:42:20Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":29.76,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":70.31,"PSucQ":null,"TDis":-191.41,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":120.52,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.94,"AmpPhB":1.58,"AmpPhC":0.94,"PDis":137.56,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.69,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.92,"TRtn1Q":null,"TRtn2":20.95,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":18.57,"PctSucVlvQ":null,"TSup1":21.02,"TSup1Q":null,"TSup2":20.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.936Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c03d4f57-74f4-4ec3-8461-b2a6aa62750d","EventDtm":"2025-11-27T08:42:44Z","AppDtm":"2025-11-27T08:43:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:42:44Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.89206,"GPSLongitude":79.476202,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:42:44Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":31.33,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.23,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":154.8,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":11.39,"AmpPhB":11.25,"AmpPhC":11.39,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.2,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":402.46,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.75,"TRtn1Q":null,"TRtn2":17.68,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.23,"PctSucVlvQ":null,"TSup1":18.53,"TSup1Q":null,"TSup2":18.56,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:44.939Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8e297f54-9691-449b-8e62-301fe20acb45","EventDtm":"2025-11-27T08:43:00Z","AppDtm":"2025-11-27T08:43:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:43:00Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804891,"GPSLongitude":77.662297,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:43:00Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":23.81,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":95.9,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.96,"AmpPhB":10.54,"AmpPhC":10.96,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.99,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.34,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.39,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.35,"TRtn1Q":null,"TRtn2":5.35,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":2.9,"PctSucVlvQ":null,"TSup1":5.04,"TSup1Q":null,"TSup2":5.06,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:45.033Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6fe48e02-6dce-4b09-a0ae-312261e72690","EventDtm":"2025-11-27T08:44:54Z","AppDtm":"2025-11-27T08:45:10Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:44:54Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":12.804887,"GPSLongitude":77.662284,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:44:54Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.78,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":97.45,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.37,"AmpPhB":11,"AmpPhC":11.37,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.1,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.77,"TRtn1Q":null,"TRtn2":5.79,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.82,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:45.063Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f9a0c53d-b8b8-4bb6-9ec4-57b5110df232","EventDtm":"2025-11-27T08:48:09Z","AppDtm":"2025-11-27T08:48:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:48:09Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.572075,"GPSLongitude":78.515111,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"230807317","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:45.066Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d37e79db-9bb8-4269-a705-f07d905f009d","EventDtm":"2025-11-27T08:54:55Z","AppDtm":"2025-11-27T08:55:10Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T08:54:55Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.804936,"GPSLongitude":77.662277,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T08:54:55Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.73,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":95.88,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.17,"AmpPhB":10.68,"AmpPhC":11.17,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.59,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.02,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.75,"TRtn1Q":null,"TRtn2":5.76,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.62,"PctSucVlvQ":null,"TSup1":5.04,"TSup1Q":null,"TSup2":4.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T08:58:45.068Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":24,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"de26e194-f204-4851-9af8-c65ab21c5285","EventDtm":"2025-11-27T10:38:23Z","AppDtm":"2025-11-27T08:56:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T10:38:23Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":6807,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
   </si>
 </sst>
 </file>
@@ -564,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1319,6 +1331,70 @@
         <v>54</v>
       </c>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
feat: Implement comprehensive client management and PM system
- Add PM fields migration for containers (last_pm_date, next_pm_due_date, pm_frequency_days, pm_status)
- Fix client authentication flow with password reset requirement
- Implement secure client onboarding with email credentials
- Add user management fixes and role-based access control
- Resolve Orbcomm integration column errors
- Update admin user management interface
- Add comprehensive client data deletion with cascade handling
- Implement force password reset page for new clients
- Add PM fields to database schema and migration tools
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="55">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,142 +43,139 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-27T09:14:27.656Z</t>
+    <t>2025-11-27T11:44:00.451Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"709f92cc-9ca0-409f-8bfa-7e8c53268a1a","EventDtm":"2025-11-27T09:08:23Z","AppDtm":"2025-11-27T09:10:12Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:08:23Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.824872,"GPSLongitude":78.131479,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.1,"BatteryVoltage":8,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:08:23Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":31.88,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":77.1,"TDisQ":null,"FreqComp":null,"TSuc":-22.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1140,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":393.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.59,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:14:27.671Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6d127935-8ae4-4240-8442-399360435d59","EventDtm":"2025-11-27T09:10:19Z","AppDtm":"2025-11-27T09:10:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:10:19Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.66159,"GPSLongitude":83.089126,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:10:19Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":60,"PSucQ":"asProvided","TDis":46.4,"TDisQ":null,"FreqComp":null,"TSuc":-12.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1070,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":370.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":"OOR","TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1b4ddbd3-ba64-44bc-a272-4bd1f9ba3dca","EventDtm":"2025-11-27T09:11:16Z","AppDtm":"2025-11-27T09:11:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:11:16Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.537106,"GPSLongitude":78.175748,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":28.1,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:11:16Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":29.87,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":134.52,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":9.41,"AmpPhB":10.74,"AmpPhC":9.41,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.67,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":9.36,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":399.12,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.39,"TRtn1Q":null,"TRtn2":-17.42,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.31,"TSup1Q":null,"TSup2":-31.54,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:14:27.687Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1bc7bbd5-f9b7-41e7-bf63-0f885c956cb7","EventDtm":"2025-11-27T09:13:33Z","AppDtm":"2025-11-27T09:13:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:13:33Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.679084,"GPSLongitude":78.720291,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":41,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:13:33Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":28.32,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-181.64,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":150.55,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.07,"AmpPhB":10.79,"AmpPhC":11.07,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.44,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.58,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":407.44,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.99,"TRtn1Q":null,"TRtn2":4.99,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.46,"PctSucVlvQ":null,"TSup1":3.95,"TSup1Q":null,"TSup2":3.97,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:15:14.270Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"eadbeb24-9ac1-496d-aaec-252c11bc4480","EventDtm":"2025-11-27T09:14:58Z","AppDtm":"2025-11-27T09:15:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:14:58Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.80501,"GPSLongitude":77.662228,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:14:58Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.71,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":97.68,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.57,"AmpPhB":11.28,"AmpPhC":11.57,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.18,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.34,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.76,"TRtn1Q":null,"TRtn2":5.77,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.67,"PctSucVlvQ":null,"TSup1":4.92,"TSup1Q":null,"TSup2":4.87,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:18:29.675Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6177a420-fe17-4ef9-83f4-13fbf272d000","EventDtm":"2025-11-27T09:18:13Z","AppDtm":"2025-11-27T09:18:29Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:18:13Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.8919,"GPSLongitude":79.475974,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":false,"ExtPowerVoltage":3.5,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:20:11.703Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a159cbb2-a2a8-4dc7-abc4-ddb1bd73925b","EventDtm":"2025-11-27T09:19:56Z","AppDtm":"2025-11-27T09:20:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:19:56Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":15.479559,"GPSLongitude":73.969693,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:19:56Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":31.27,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":182.65,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":11.82,"AmpPhB":11.29,"AmpPhC":11.82,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":7.22,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":86.86,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.75,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.09,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":6.69,"TRtn1Q":null,"TRtn2":6.69,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":12.39,"PctSucVlvQ":null,"TSup1":4.71,"TSup1Q":null,"TSup2":4.73,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:20:41.838Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ee311ca4-f8d4-4c7c-ba77-6061a84c710c","EventDtm":"2025-11-27T09:20:26Z","AppDtm":"2025-11-27T09:20:42Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:20:26Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891876,"GPSLongitude":79.476006,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:20:26Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":30.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":230,"PSucQ":"asProvided","TDis":59.7,"TDisQ":null,"FreqComp":null,"TSuc":2.9,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":880,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":3.69,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":6.5,"TRtn1Q":null,"TRtn2":37.7,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:20:58.296Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d948b6cf-a52f-4d53-b6b8-4bad6ec8eb92","EventDtm":"2025-11-27T09:20:42Z","AppDtm":"2025-11-27T09:20:58Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:20:42Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":26.310543,"GPSLongitude":91.717649,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:20:42Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":77.4,"TDisQ":null,"FreqComp":null,"TSuc":-23.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1030,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":73,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":390.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":96.95,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:23:02.398Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"31c4b827-145e-4ec8-939a-35e0beebf629","EventDtm":"2025-11-27T09:22:47Z","AppDtm":"2025-11-27T09:23:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:22:47Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.533288,"GPSLongitude":78.433076,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8.1,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:22:47Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":30.12,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":190,"PSucQ":"asProvided","TDis":62.3,"TDisQ":null,"FreqComp":null,"TSuc":19.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1140,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":411.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.81,"TRtn1Q":null,"TRtn2":136.4,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":104.27,"PctSucVlvQ":null,"TSup1":4.69,"TSup1Q":null,"TSup2":5.3,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:23:29.090Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"88b717a8-184f-4c74-9432-77334285c39a","EventDtm":"2025-11-27T09:23:12Z","AppDtm":"2025-11-27T09:23:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:23:12Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.516029,"GPSLongitude":82.981179,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:23:12Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":29.25,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.09,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.67,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.57,"AmpPhB":10.82,"AmpPhC":11.57,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.37,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.1,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.63,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.04,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.81,"TRtn1Q":null,"TRtn2":3.85,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":5.74,"PctSucVlvQ":null,"TSup1":3.05,"TSup1Q":null,"TSup2":3.11,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:24:26.467Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2cba9932-c7e4-4089-91f2-a104d05c2191","EventDtm":"2025-11-27T09:24:10Z","AppDtm":"2025-11-27T09:24:26Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:24:10Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891876,"GPSLongitude":79.476015,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:24:10Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":270,"PSucQ":"asProvided","TDis":41.2,"TDisQ":null,"FreqComp":null,"TSuc":6.6,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":590,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":38,"PctExpVlvQ":null,"TEvap":6.62,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":403.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":7,"TRtn1Q":null,"TRtn2":38.6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":6.69,"TSup1Q":null,"TSup2":6.4,"TSup2Q":null,"AmpTotalDraw":3,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:24:49.200Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4b213a5a-c3e4-4210-a8ef-81283aff6c0f","EventDtm":"2025-11-27T09:24:32Z","AppDtm":"2025-11-27T09:24:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:24:32Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.547776,"GPSLongitude":78.380506,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:25:57.256Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"08dffa83-e5cc-4944-aa1f-36f96c33a906","EventDtm":"2025-11-27T09:25:34Z","AppDtm":"2025-11-27T09:25:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:25:34Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":21.735536,"GPSLongitude":72.62897,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:25:34Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":34.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":214.6,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":14.33,"AmpPhB":14.04,"AmpPhC":14.33,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.44,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89.02,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":439.59,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.71,"TRtn1Q":null,"TRtn2":15.67,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.37,"PctSucVlvQ":null,"TSup1":14.93,"TSup1Q":null,"TSup2":15.11,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:26:21.871Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a365fba9-eb8d-4478-a657-2921b3466b6b","EventDtm":"2025-11-27T09:24:56Z","AppDtm":"2025-11-27T09:25:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:24:56Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804989,"GPSLongitude":77.662222,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:24:56Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.37,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":94.81,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.21,"AmpPhB":10.93,"AmpPhC":11.21,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.23,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.37,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.07,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.8,"TRtn1Q":null,"TRtn2":5.81,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.94,"PctSucVlvQ":null,"TSup1":5.08,"TSup1Q":null,"TSup2":5.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:27:25.196Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"141c2606-cf53-43c5-8bd4-fc2699b88fe9","EventDtm":"2025-11-27T09:27:05Z","AppDtm":"2025-11-27T09:27:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:27:05Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.516196,"GPSLongitude":82.962358,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957963","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:27:05Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":28.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":82.5,"TDisQ":null,"FreqComp":null,"TSuc":-11.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":52,"PctExpVlvQ":null,"TEvap":22.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":382,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.7,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:30:14.931Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2f140ac8-0759-45ab-ad4d-509d1a99d0c9","EventDtm":"2025-11-27T09:29:55Z","AppDtm":"2025-11-27T09:30:13Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:29:55Z","DeviceID":"JSGA623040302","GPSLockState":"UNLOCKED","GPSSatelliteCount":11,"GPSLastLock":8,"GPSLatitude":19.252891,"GPSLongitude":73.016487,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:30:47.395Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"db99f8a4-beea-4966-8de2-46073d55c19f","EventDtm":"2025-11-27T09:30:31Z","AppDtm":"2025-11-27T09:30:47Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:30:31Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":16.891875,"GPSLongitude":79.475967,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":false,"ExtPowerVoltage":7.6,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:31:42.633Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a0222ab3-0198-488e-94d7-20a76f6e59a6","EventDtm":"2025-11-27T09:31:21Z","AppDtm":"2025-11-27T09:31:39Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:31:21Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":28.3647,"GPSLongitude":75.581313,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-83","ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:31:21Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":23,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":35,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":7.5,"AmpPhB":8.5,"AmpPhC":8.7,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17.1,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.3,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":6.6,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:35:11.479Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"20569417-ef38-44dd-b2e0-752e14846b13","EventDtm":"2025-11-27T09:34:56Z","AppDtm":"2025-11-27T09:35:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:34:56Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.804995,"GPSLongitude":77.662179,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:34:56Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.39,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":94.87,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.61,"AmpPhB":11.12,"AmpPhC":11.61,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.53,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.01,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.8,"TRtn1Q":null,"TRtn2":5.82,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.35,"PctSucVlvQ":null,"TSup1":4.99,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:36:02.683Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"178b2d8c-e62d-40a6-8374-7bf6a4b18ed2","EventDtm":"2025-11-27T09:35:46Z","AppDtm":"2025-11-27T09:36:02Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:35:46Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.572252,"GPSLongitude":78.51498,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323424","RSSI":"-69","ExtPower":false,"ExtPowerVoltage":4.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:36:53.369Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d8a3c1be-3611-4ad5-adc9-8c8a792e65bb","EventDtm":"2025-11-27T09:34:17Z","AppDtm":"2025-11-27T09:36:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:34:17Z","DeviceID":"JSGA622340507","GPSLockState":"LOCKED","GPSSatelliteCount":9,"GPSLastLock":0,"GPSLatitude":17.501785,"GPSLongitude":82.962453,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136287","RSSI":"-73","ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.7,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6616969","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T09:37:36.579Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"da8dd501-58da-4019-b643-91e057038efa","EventDtm":"2025-11-27T09:37:15Z","AppDtm":"2025-11-27T09:37:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T09:37:15Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.657912,"GPSLongitude":83.101838,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T09:37:15Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":30.06,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":70.04,"PSucQ":null,"TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":114.5,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.93,"AmpPhB":1.55,"AmpPhC":0.93,"PDis":114.59,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.81,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":423.32,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.54,"TRtn1Q":null,"TRtn2":20.59,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":18.25,"PctSucVlvQ":null,"TSup1":20.06,"TSup1Q":null,"TSup2":20.14,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0e4b51c8-0977-42ff-9d65-f0366b26404b","EventDtm":"2025-11-27T11:10:18Z","AppDtm":"2025-11-27T11:10:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:10:18Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661606,"GPSLongitude":83.089151,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:10:18Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":29.62,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":47.2,"TDisQ":null,"FreqComp":null,"TSuc":-12.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1080,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":370.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":99.39,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.505Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a436a668-0c5c-4920-89be-8e4803e23387","EventDtm":"2025-11-27T11:11:09Z","AppDtm":"2025-11-27T11:11:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:11:09Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.537175,"GPSLongitude":78.17565,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":28.1,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:11:09Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":28.81,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":192.79,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":9.01,"AmpPhB":10.5,"AmpPhC":9.01,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.49,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":8.58,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":397.43,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.59,"TRtn1Q":null,"TRtn2":-17.62,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.33,"TSup1Q":null,"TSup2":-31.59,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.510Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1315c341-0a3e-42af-9831-ce66a20559fa","EventDtm":"2025-11-27T11:13:49Z","AppDtm":"2025-11-27T11:14:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:13:49Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.679111,"GPSLongitude":78.72017,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:13:49Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":26.68,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.42,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":142.67,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.27,"AmpPhB":10.79,"AmpPhC":11.27,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.39,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.66,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.66,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.93,"TRtn1Q":null,"TRtn2":4.93,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.39,"PctSucVlvQ":null,"TSup1":3.97,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.520Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ce21236a-e35b-4300-a5f3-16ce806aa2af","EventDtm":"2025-11-27T11:14:59Z","AppDtm":"2025-11-27T11:15:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:14:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.80506,"GPSLongitude":77.662238,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:14:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.89,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":91.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.22,"AmpPhB":10.86,"AmpPhC":11.22,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.68,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.75,"TRtn1Q":null,"TRtn2":5.77,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.01,"PctSucVlvQ":null,"TSup1":5.03,"TSup1Q":null,"TSup2":4.97,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.646Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ddd3e689-9a6a-49f0-9c88-43832606f104","EventDtm":"2025-11-27T11:18:47Z","AppDtm":"2025-11-27T11:19:57Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:18:47Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":28.678605,"GPSLongitude":77.599696,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":7.8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:18:47Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":23.07,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":71.19,"PSucQ":null,"TDis":30.29,"TDisQ":null,"FreqComp":null,"TSuc":22.12,"TSucQ":null,"MCond":0,"PCond":307.63,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Configuration","SnCtrl":"04475864","AmpPhA":0,"AmpPhB":0,"AmpPhC":0,"PDis":82.39,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":22.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":53.72,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.8,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":22.29,"TRtn1Q":null,"TRtn2":22.27,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":20.56,"TSup1Q":null,"TSup2":20.42,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.664Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4950d42f-bb64-41d1-a385-e5f3f3720f4d","EventDtm":"2025-11-27T11:20:03Z","AppDtm":"2025-11-27T11:20:17Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:20:03Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":15.479507,"GPSLongitude":73.969716,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082161","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:20:03Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.18,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":156.47,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.95,"AmpPhB":10.25,"AmpPhC":10.95,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.01,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89.25,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.11,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.68,"TRtn1Q":null,"TRtn2":5.7,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.4,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.673Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f00fc88-655f-4f49-a3e6-e1601041af7e","EventDtm":"2025-11-27T11:22:54Z","AppDtm":"2025-11-27T11:23:08Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:22:54Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.533259,"GPSLongitude":78.433081,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:22:54Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":28.19,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":49.6,"TDisQ":null,"FreqComp":null,"TSuc":6.2,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":413.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.69,"TRtn1Q":null,"TRtn2":136.4,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":4.88,"TSup1Q":null,"TSup2":4.9,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.679Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"741b50a6-a6e2-456b-b167-1416f05b0500","EventDtm":"2025-11-27T11:23:05Z","AppDtm":"2025-11-27T11:23:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:23:05Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.515871,"GPSLongitude":82.981198,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:23:05Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":27.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-195.7,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":134.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.65,"AmpPhB":10.88,"AmpPhC":11.65,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.1,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.59,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.68,"TRtn1Q":null,"TRtn2":3.72,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.2,"PctSucVlvQ":null,"TSup1":2.97,"TSup1Q":null,"TSup2":3.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.686Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4e78ff79-e80b-49a5-aa5c-430d4d32466f","EventDtm":"2025-11-27T11:24:49Z","AppDtm":"2025-11-27T11:25:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:24:49Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.547759,"GPSLongitude":78.380603,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8.1,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.691Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"10d26ec2-9a70-4360-ac23-fcb90c398c9c","EventDtm":"2025-11-27T11:25:04Z","AppDtm":"2025-11-27T11:25:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:25:04Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804989,"GPSLongitude":77.66223,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:25:04Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.69,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":101.42,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.52,"AmpPhB":10.91,"AmpPhC":11.52,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.17,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.04,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.73,"TRtn1Q":null,"TRtn2":5.74,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.86,"PctSucVlvQ":null,"TSup1":4.97,"TSup1Q":null,"TSup2":4.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.700Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"916aba94-a5f9-4861-9f7e-d0fb8574aca6","EventDtm":"2025-11-27T11:25:31Z","AppDtm":"2025-11-27T11:26:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:25:31Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":21.735604,"GPSLongitude":72.628937,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:25:31Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":32.79,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":194.67,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":14.48,"AmpPhB":14.13,"AmpPhC":14.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.34,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":439.92,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.61,"TRtn1Q":null,"TRtn2":15.57,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.3,"PctSucVlvQ":null,"TSup1":14.93,"TSup1Q":null,"TSup2":15.12,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.707Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"363ebb72-6290-486f-99ce-61bafb17e84d","EventDtm":"2025-11-27T11:27:18Z","AppDtm":"2025-11-27T11:27:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:27:18Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.516211,"GPSLongitude":82.962407,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957963","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:27:18Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":26.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":85.3,"TDisQ":null,"FreqComp":null,"TSuc":-10.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":52,"PctExpVlvQ":null,"TEvap":22.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":385.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.6,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.67,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.709Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"26019181-91da-424e-989d-e5afba241a88","EventDtm":"2025-11-27T11:30:46Z","AppDtm":"2025-11-27T11:31:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:30:46Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":2,"GPSLatitude":19.252943,"GPSLongitude":73.016489,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.711Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"57805939-2709-4403-a366-a934ddd07105","EventDtm":"2025-11-27T11:31:37Z","AppDtm":"2025-11-27T11:31:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:31:37Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":28.364693,"GPSLongitude":75.581333,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"144900619","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:31:37Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":21,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":35,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":6.3,"AmpPhB":7.1,"AmpPhC":7.2,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":8.7,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.713Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9b9a09e7-5976-4167-bdb4-5829df14675b","EventDtm":"2025-11-27T11:33:04Z","AppDtm":"2025-11-27T11:33:37Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:33:04Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":28.678712,"GPSLongitude":77.599821,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"128143137","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":6.5,"BatteryVoltage":7.9,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.717Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6e1e710b-2bd8-4678-b8c5-dbbc2f37074e","EventDtm":"2025-11-27T11:34:59Z","AppDtm":"2025-11-27T11:35:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:34:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804959,"GPSLongitude":77.662233,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:34:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.77,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":92.59,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.47,"AmpPhB":11.14,"AmpPhC":11.47,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.13,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.66,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.7,"TRtn1Q":null,"TRtn2":5.71,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.94,"PctSucVlvQ":null,"TSup1":4.91,"TSup1Q":null,"TSup2":4.84,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.720Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"798eca91-746f-40c2-b2b6-83e817d4e070","EventDtm":"2025-11-27T11:36:57Z","AppDtm":"2025-11-27T11:37:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:36:57Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657974,"GPSLongitude":83.101707,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:36:57Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":27.35,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":71.75,"PSucQ":null,"TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":102.05,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.91,"AmpPhB":1.52,"AmpPhC":0.91,"PDis":101.89,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.02,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.73,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.84,"TRtn1Q":null,"TRtn2":20.9,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":20.51,"PctSucVlvQ":null,"TSup1":21.21,"TSup1Q":null,"TSup2":21.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.723Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"032e4b41-c60c-40b6-bb94-a7dcc1ec99ba","EventDtm":"2025-11-27T11:37:48Z","AppDtm":"2025-11-27T11:38:35Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:37:48Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.606166,"GPSLongitude":80.723641,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.725Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"53a28523-5a33-4cd2-bb82-79a89b2c5b06","EventDtm":"2025-11-27T11:38:50Z","AppDtm":"2025-11-27T11:39:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:38:50Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":16.892092,"GPSLongitude":79.476263,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:38:50Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":28.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":83.1,"TDisQ":null,"FreqComp":null,"TSuc":-29.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":21,"PctExpVlvQ":null,"TEvap":-0.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":406.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.59,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.861Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"46198e8a-c86c-4eae-a6d0-ab94b285a3ea","EventDtm":"2025-11-27T11:38:48Z","AppDtm":"2025-11-27T11:39:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:38:48Z","DeviceID":"JSGA623040314","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":19.252949,"GPSLongitude":73.016614,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:38:48Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":25.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-188.67,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.43,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.9,"AmpPhB":11.01,"AmpPhC":10.9,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.86,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":403.43,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.35,"TRtn1Q":null,"TRtn2":5.49,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":3.6,"PctSucVlvQ":null,"TSup1":8.2,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.904Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ea42ba80-ff48-435c-87a3-955a0b4e0f3a","EventDtm":"2025-11-27T11:40:36Z","AppDtm":"2025-11-27T11:40:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:40:36Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":9,"GPSLastLock":19,"GPSLatitude":17.548033,"GPSLongitude":78.3806,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":33.2,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T11:44:00.907Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4683e802-dd00-4882-9f62-d45580eff059","EventDtm":"2025-11-27T11:42:48Z","AppDtm":"2025-11-27T11:43:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:42:48Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657819,"GPSLongitude":83.101808,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":7.9,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:42:48Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":27.63,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":64.93,"PSucQ":null,"TDis":-188.28,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":122.97,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.91,"AmpPhB":1.54,"AmpPhC":0.91,"PDis":137.51,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.25,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":406.58,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20,"TRtn1Q":null,"TRtn2":20.01,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":20.28,"PctSucVlvQ":null,"TSup1":18.55,"TSup1Q":null,"TSup2":18.65,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
   </si>
 </sst>
 </file>
@@ -567,7 +564,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -684,7 +681,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -711,12 +708,12 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -743,12 +740,12 @@
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -775,12 +772,12 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -807,12 +804,12 @@
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -839,12 +836,12 @@
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -871,12 +868,12 @@
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -903,12 +900,12 @@
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -935,12 +932,12 @@
         <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -967,12 +964,12 @@
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -999,12 +996,12 @@
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -1031,12 +1028,12 @@
         <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1063,12 +1060,12 @@
         <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -1095,12 +1092,12 @@
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -1127,12 +1124,12 @@
         <v>11</v>
       </c>
       <c r="J17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -1159,12 +1156,12 @@
         <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -1191,12 +1188,12 @@
         <v>11</v>
       </c>
       <c r="J19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1223,12 +1220,12 @@
         <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -1255,12 +1252,12 @@
         <v>11</v>
       </c>
       <c r="J21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -1287,12 +1284,12 @@
         <v>11</v>
       </c>
       <c r="J22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -1319,39 +1316,7 @@
         <v>11</v>
       </c>
       <c r="J23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: resolve user management 401 errors and email service timeout issues
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,139 +43,67 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-27T11:44:00.451Z</t>
+    <t>2025-11-27T13:15:00.746Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0e4b51c8-0977-42ff-9d65-f0366b26404b","EventDtm":"2025-11-27T11:10:18Z","AppDtm":"2025-11-27T11:10:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:10:18Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661606,"GPSLongitude":83.089151,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:10:18Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":29.62,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":47.2,"TDisQ":null,"FreqComp":null,"TSuc":-12.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1080,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":370.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":99.39,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.505Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a436a668-0c5c-4920-89be-8e4803e23387","EventDtm":"2025-11-27T11:11:09Z","AppDtm":"2025-11-27T11:11:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:11:09Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.537175,"GPSLongitude":78.17565,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":28.1,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:11:09Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":28.81,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":192.79,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":9.01,"AmpPhB":10.5,"AmpPhC":9.01,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.49,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":8.58,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":397.43,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.59,"TRtn1Q":null,"TRtn2":-17.62,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.33,"TSup1Q":null,"TSup2":-31.59,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.510Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1315c341-0a3e-42af-9831-ce66a20559fa","EventDtm":"2025-11-27T11:13:49Z","AppDtm":"2025-11-27T11:14:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:13:49Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.679111,"GPSLongitude":78.72017,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:13:49Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":26.68,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.42,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":142.67,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.27,"AmpPhB":10.79,"AmpPhC":11.27,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.39,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.66,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.66,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.93,"TRtn1Q":null,"TRtn2":4.93,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.39,"PctSucVlvQ":null,"TSup1":3.97,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.520Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ce21236a-e35b-4300-a5f3-16ce806aa2af","EventDtm":"2025-11-27T11:14:59Z","AppDtm":"2025-11-27T11:15:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:14:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.80506,"GPSLongitude":77.662238,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:14:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.89,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":91.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.22,"AmpPhB":10.86,"AmpPhC":11.22,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.68,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.75,"TRtn1Q":null,"TRtn2":5.77,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.01,"PctSucVlvQ":null,"TSup1":5.03,"TSup1Q":null,"TSup2":4.97,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.646Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ddd3e689-9a6a-49f0-9c88-43832606f104","EventDtm":"2025-11-27T11:18:47Z","AppDtm":"2025-11-27T11:19:57Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:18:47Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":28.678605,"GPSLongitude":77.599696,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":7.8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:18:47Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":23.07,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":71.19,"PSucQ":null,"TDis":30.29,"TDisQ":null,"FreqComp":null,"TSuc":22.12,"TSucQ":null,"MCond":0,"PCond":307.63,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Configuration","SnCtrl":"04475864","AmpPhA":0,"AmpPhB":0,"AmpPhC":0,"PDis":82.39,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":22.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":53.72,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.8,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":22.29,"TRtn1Q":null,"TRtn2":22.27,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":20.56,"TSup1Q":null,"TSup2":20.42,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.664Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4950d42f-bb64-41d1-a385-e5f3f3720f4d","EventDtm":"2025-11-27T11:20:03Z","AppDtm":"2025-11-27T11:20:17Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:20:03Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":15.479507,"GPSLongitude":73.969716,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082161","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:20:03Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.18,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":156.47,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.95,"AmpPhB":10.25,"AmpPhC":10.95,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.01,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":89.25,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.11,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.68,"TRtn1Q":null,"TRtn2":5.7,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.4,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.673Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f00fc88-655f-4f49-a3e6-e1601041af7e","EventDtm":"2025-11-27T11:22:54Z","AppDtm":"2025-11-27T11:23:08Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:22:54Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.533259,"GPSLongitude":78.433081,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:22:54Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":28.19,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":49.6,"TDisQ":null,"FreqComp":null,"TSuc":6.2,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":413.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.69,"TRtn1Q":null,"TRtn2":136.4,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":4.88,"TSup1Q":null,"TSup2":4.9,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.679Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"741b50a6-a6e2-456b-b167-1416f05b0500","EventDtm":"2025-11-27T11:23:05Z","AppDtm":"2025-11-27T11:23:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:23:05Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.515871,"GPSLongitude":82.981198,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:23:05Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":27.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-195.7,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":134.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.65,"AmpPhB":10.88,"AmpPhC":11.65,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.1,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.59,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.68,"TRtn1Q":null,"TRtn2":3.72,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.2,"PctSucVlvQ":null,"TSup1":2.97,"TSup1Q":null,"TSup2":3.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.686Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4e78ff79-e80b-49a5-aa5c-430d4d32466f","EventDtm":"2025-11-27T11:24:49Z","AppDtm":"2025-11-27T11:25:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:24:49Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.547759,"GPSLongitude":78.380603,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8.1,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.691Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"10d26ec2-9a70-4360-ac23-fcb90c398c9c","EventDtm":"2025-11-27T11:25:04Z","AppDtm":"2025-11-27T11:25:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:25:04Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804989,"GPSLongitude":77.66223,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:25:04Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.69,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":101.42,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.52,"AmpPhB":10.91,"AmpPhC":11.52,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.17,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.04,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.73,"TRtn1Q":null,"TRtn2":5.74,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.86,"PctSucVlvQ":null,"TSup1":4.97,"TSup1Q":null,"TSup2":4.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.700Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"916aba94-a5f9-4861-9f7e-d0fb8574aca6","EventDtm":"2025-11-27T11:25:31Z","AppDtm":"2025-11-27T11:26:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:25:31Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":21.735604,"GPSLongitude":72.628937,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:25:31Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":32.79,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":194.67,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":14.48,"AmpPhB":14.13,"AmpPhC":14.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.34,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":439.92,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.61,"TRtn1Q":null,"TRtn2":15.57,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.3,"PctSucVlvQ":null,"TSup1":14.93,"TSup1Q":null,"TSup2":15.12,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.707Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"363ebb72-6290-486f-99ce-61bafb17e84d","EventDtm":"2025-11-27T11:27:18Z","AppDtm":"2025-11-27T11:27:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:27:18Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.516211,"GPSLongitude":82.962407,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957963","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:27:18Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":26.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":85.3,"TDisQ":null,"FreqComp":null,"TSuc":-10.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":52,"PctExpVlvQ":null,"TEvap":22.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":385.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.6,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.67,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.709Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"26019181-91da-424e-989d-e5afba241a88","EventDtm":"2025-11-27T11:30:46Z","AppDtm":"2025-11-27T11:31:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:30:46Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":2,"GPSLatitude":19.252943,"GPSLongitude":73.016489,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.711Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"57805939-2709-4403-a366-a934ddd07105","EventDtm":"2025-11-27T11:31:37Z","AppDtm":"2025-11-27T11:31:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:31:37Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":28.364693,"GPSLongitude":75.581333,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"144900619","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:31:37Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":21,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":35,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":6.3,"AmpPhB":7.1,"AmpPhC":7.2,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":8.7,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.713Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9b9a09e7-5976-4167-bdb4-5829df14675b","EventDtm":"2025-11-27T11:33:04Z","AppDtm":"2025-11-27T11:33:37Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:33:04Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":28.678712,"GPSLongitude":77.599821,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"128143137","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":6.5,"BatteryVoltage":7.9,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.717Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6e1e710b-2bd8-4678-b8c5-dbbc2f37074e","EventDtm":"2025-11-27T11:34:59Z","AppDtm":"2025-11-27T11:35:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:34:59Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804959,"GPSLongitude":77.662233,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:34:59Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.77,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":92.59,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.47,"AmpPhB":11.14,"AmpPhC":11.47,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.13,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.66,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.7,"TRtn1Q":null,"TRtn2":5.71,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.94,"PctSucVlvQ":null,"TSup1":4.91,"TSup1Q":null,"TSup2":4.84,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.720Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"798eca91-746f-40c2-b2b6-83e817d4e070","EventDtm":"2025-11-27T11:36:57Z","AppDtm":"2025-11-27T11:37:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:36:57Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657974,"GPSLongitude":83.101707,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:36:57Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":27.35,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":71.75,"PSucQ":null,"TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":102.05,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.91,"AmpPhB":1.52,"AmpPhC":0.91,"PDis":101.89,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.02,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.73,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.84,"TRtn1Q":null,"TRtn2":20.9,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":20.51,"PctSucVlvQ":null,"TSup1":21.21,"TSup1Q":null,"TSup2":21.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.723Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"032e4b41-c60c-40b6-bb94-a7dcc1ec99ba","EventDtm":"2025-11-27T11:37:48Z","AppDtm":"2025-11-27T11:38:35Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:37:48Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":26.606166,"GPSLongitude":80.723641,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.725Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"53a28523-5a33-4cd2-bb82-79a89b2c5b06","EventDtm":"2025-11-27T11:38:50Z","AppDtm":"2025-11-27T11:39:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:38:50Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":16.892092,"GPSLongitude":79.476263,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:38:50Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":28.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":83.1,"TDisQ":null,"FreqComp":null,"TSuc":-29.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":21,"PctExpVlvQ":null,"TEvap":-0.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":406.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.59,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.861Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"46198e8a-c86c-4eae-a6d0-ab94b285a3ea","EventDtm":"2025-11-27T11:38:48Z","AppDtm":"2025-11-27T11:39:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:38:48Z","DeviceID":"JSGA623040314","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":19.252949,"GPSLongitude":73.016614,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:38:48Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":25.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-188.67,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.43,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.9,"AmpPhB":11.01,"AmpPhC":10.9,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.86,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":403.43,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.35,"TRtn1Q":null,"TRtn2":5.49,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":3.6,"PctSucVlvQ":null,"TSup1":8.2,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.904Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ea42ba80-ff48-435c-87a3-955a0b4e0f3a","EventDtm":"2025-11-27T11:40:36Z","AppDtm":"2025-11-27T11:40:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:40:36Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":9,"GPSLastLock":19,"GPSLatitude":17.548033,"GPSLongitude":78.3806,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":33.2,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T11:44:00.907Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4683e802-dd00-4882-9f62-d45580eff059","EventDtm":"2025-11-27T11:42:48Z","AppDtm":"2025-11-27T11:43:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T11:42:48Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657819,"GPSLongitude":83.101808,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":7.9,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T11:42:48Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":27.63,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":64.93,"PSucQ":null,"TDis":-188.28,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":122.97,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.91,"AmpPhB":1.54,"AmpPhC":0.91,"PDis":137.51,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.25,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":406.58,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20,"TRtn1Q":null,"TRtn2":20.01,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":20.28,"PctSucVlvQ":null,"TSup1":18.55,"TSup1Q":null,"TSup2":18.65,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d74318a2-e69a-4a80-85f2-2d89cb19662d","EventDtm":"2025-11-27T12:59:44Z","AppDtm":"2025-11-27T13:00:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T12:59:44Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.539016,"GPSLongitude":78.178353,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.4,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T12:59:44Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":26.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":112.6,"TDisQ":null,"FreqComp":null,"TSuc":-35.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:00.998Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"09f1e680-1dd7-4dac-9818-58bd20690ea0","EventDtm":"2025-11-27T13:01:29Z","AppDtm":"2025-11-27T13:01:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:01:29Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533149,"GPSLongitude":78.433604,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:01:29Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":25.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":71.8,"TDisQ":null,"FreqComp":null,"TSuc":-30.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":418.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6.2,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:01.422Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"35b4b8b4-29e0-407f-a66b-85af65516e97","EventDtm":"2025-11-27T13:02:23Z","AppDtm":"2025-11-27T13:02:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:02:23Z","DeviceID":"JSGA623040321","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.816183,"GPSLongitude":77.687294,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9057","CID":"180498700","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6617250","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:01.676Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1d989149-95b7-40d7-b424-e5d22bd41a94","EventDtm":"2025-11-27T13:04:53Z","AppDtm":"2025-11-27T13:05:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:04:53Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":26.644409,"GPSLongitude":88.467959,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8.1,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:04:53Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":23.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-50,"PSucQ":"asProvided","TDis":96.8,"TDisQ":null,"FreqComp":null,"TSuc":-29.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":790,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":12,"PctExpVlvQ":null,"TEvap":-0.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.81,"TRtn1Q":null,"TRtn2":1.6,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.7,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:02.122Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7df7cac5-50df-4a89-bf26-f8c3322a4554","EventDtm":"2025-11-27T13:05:03Z","AppDtm":"2025-11-27T13:05:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:05:03Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.80499,"GPSLongitude":77.662225,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:05:03Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":29.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":88.22,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.66,"AmpPhB":11.27,"AmpPhC":11.66,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.71,"TRtn1Q":null,"TRtn2":5.72,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.58,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:02.486Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c74ecaba-9185-482a-8953-b954c8f22456","EventDtm":"2025-11-27T13:08:48Z","AppDtm":"2025-11-27T13:09:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:08:48Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":16.824945,"GPSLongitude":78.131517,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:08:48Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":26.12,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":72.5,"TDisQ":null,"FreqComp":null,"TSuc":-26.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.81,"TRtn1Q":null,"TRtn2":4.6,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:02.782Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"14d7f88e-0174-46bf-b976-47340e246acd","EventDtm":"2025-11-27T13:10:18Z","AppDtm":"2025-11-27T13:10:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:10:18Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.661607,"GPSLongitude":83.089135,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.8,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:10:18Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":42.9,"TDisQ":null,"FreqComp":null,"TSuc":-15.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":970,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":373.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":92.68,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:02.930Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0917fa97-7d41-4329-a671-d94bb2b525b6","EventDtm":"2025-11-27T13:11:05Z","AppDtm":"2025-11-27T13:11:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:11:05Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.537024,"GPSLongitude":78.175741,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:11:05Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":26.59,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":153.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":10.05,"AmpPhB":11.44,"AmpPhC":10.05,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.58,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":8.31,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.36,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.81,"TRtn1Q":null,"TRtn2":-17.82,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.58,"TSup1Q":null,"TSup2":-31.8,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:03.047Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6420c9e7-b35a-4bcd-ae2f-4007014d9dfa","EventDtm":"2025-11-27T13:14:12Z","AppDtm":"2025-11-27T13:14:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:14:12Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.679043,"GPSLongitude":78.72014,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:14:12Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":23.58,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-181.64,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":130.59,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.3,"AmpPhB":10.85,"AmpPhC":11.3,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.43,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.79,"TRtn1Q":null,"TRtn2":4.78,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.83,"PctSucVlvQ":null,"TSup1":3.96,"TSup1Q":null,"TSup2":3.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T13:15:28.155Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6d62729e-c960-4ab8-8c28-9104c53575cf","EventDtm":"2025-11-27T13:15:09Z","AppDtm":"2025-11-27T13:15:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:15:09Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804926,"GPSLongitude":77.662245,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:15:09Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":29.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":89,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.54,"AmpPhB":11.14,"AmpPhC":11.54,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.13,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.39,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.01,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.68,"TRtn1Q":null,"TRtn2":5.7,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.41,"PctSucVlvQ":null,"TSup1":4.99,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
   </si>
 </sst>
 </file>
@@ -564,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -935,390 +863,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J23" t="s">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Merge local changes with team updates - TypeScript fixes, third-party technician helpers, and package updates
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:00.746Z</t>
+    <t>2025-11-27T13:07:24.620Z</t>
   </si>
   <si>
     <t>N/A</t>
@@ -52,58 +52,46 @@
     <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d74318a2-e69a-4a80-85f2-2d89cb19662d","EventDtm":"2025-11-27T12:59:44Z","AppDtm":"2025-11-27T13:00:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T12:59:44Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.539016,"GPSLongitude":78.178353,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.4,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T12:59:44Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":26.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":112.6,"TDisQ":null,"FreqComp":null,"TSuc":-35.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:00.998Z</t>
+    <t>2025-11-27T13:07:24.662Z</t>
   </si>
   <si>
     <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"09f1e680-1dd7-4dac-9818-58bd20690ea0","EventDtm":"2025-11-27T13:01:29Z","AppDtm":"2025-11-27T13:01:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:01:29Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533149,"GPSLongitude":78.433604,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:01:29Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":25.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":71.8,"TDisQ":null,"FreqComp":null,"TSuc":-30.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":418.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6.2,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:01.422Z</t>
+    <t>2025-11-27T13:07:24.670Z</t>
   </si>
   <si>
     <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"35b4b8b4-29e0-407f-a66b-85af65516e97","EventDtm":"2025-11-27T13:02:23Z","AppDtm":"2025-11-27T13:02:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:02:23Z","DeviceID":"JSGA623040321","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.816183,"GPSLongitude":77.687294,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9057","CID":"180498700","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6617250","LastAssetRunState":"Running"},"ReeferData":null}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:01.676Z</t>
+    <t>2025-11-27T13:07:24.674Z</t>
   </si>
   <si>
     <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1d989149-95b7-40d7-b424-e5d22bd41a94","EventDtm":"2025-11-27T13:04:53Z","AppDtm":"2025-11-27T13:05:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:04:53Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":26.644409,"GPSLongitude":88.467959,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8.1,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:04:53Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":23.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-50,"PSucQ":"asProvided","TDis":96.8,"TDisQ":null,"FreqComp":null,"TSuc":-29.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":790,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":12,"PctExpVlvQ":null,"TEvap":-0.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.81,"TRtn1Q":null,"TRtn2":1.6,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.7,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:02.122Z</t>
+    <t>2025-11-27T13:07:24.679Z</t>
   </si>
   <si>
     <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7df7cac5-50df-4a89-bf26-f8c3322a4554","EventDtm":"2025-11-27T13:05:03Z","AppDtm":"2025-11-27T13:05:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:05:03Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.80499,"GPSLongitude":77.662225,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:05:03Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":29.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":88.22,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.66,"AmpPhB":11.27,"AmpPhC":11.66,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.71,"TRtn1Q":null,"TRtn2":5.72,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.58,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:02.486Z</t>
+    <t>2025-11-27T13:09:05.762Z</t>
   </si>
   <si>
     <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c74ecaba-9185-482a-8953-b954c8f22456","EventDtm":"2025-11-27T13:08:48Z","AppDtm":"2025-11-27T13:09:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:08:48Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":16.824945,"GPSLongitude":78.131517,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:08:48Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":26.12,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":72.5,"TDisQ":null,"FreqComp":null,"TSuc":-26.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.81,"TRtn1Q":null,"TRtn2":4.6,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:02.782Z</t>
+    <t>2025-11-27T13:10:42.027Z</t>
   </si>
   <si>
     <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"14d7f88e-0174-46bf-b976-47340e246acd","EventDtm":"2025-11-27T13:10:18Z","AppDtm":"2025-11-27T13:10:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:10:18Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.661607,"GPSLongitude":83.089135,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.8,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:10:18Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":42.9,"TDisQ":null,"FreqComp":null,"TSuc":-15.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":970,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":373.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":92.68,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
   <si>
-    <t>2025-11-27T13:15:02.930Z</t>
+    <t>2025-11-27T13:11:26.371Z</t>
   </si>
   <si>
     <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0917fa97-7d41-4329-a671-d94bb2b525b6","EventDtm":"2025-11-27T13:11:05Z","AppDtm":"2025-11-27T13:11:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:11:05Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.537024,"GPSLongitude":78.175741,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:11:05Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":26.59,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":153.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":10.05,"AmpPhB":11.44,"AmpPhC":10.05,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.58,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":8.31,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.36,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.81,"TRtn1Q":null,"TRtn2":-17.82,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.58,"TSup1Q":null,"TSup2":-31.8,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:15:03.047Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6420c9e7-b35a-4bcd-ae2f-4007014d9dfa","EventDtm":"2025-11-27T13:14:12Z","AppDtm":"2025-11-27T13:14:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:14:12Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.679043,"GPSLongitude":78.72014,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:14:12Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":23.58,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-181.64,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":130.59,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.3,"AmpPhB":10.85,"AmpPhC":11.3,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.43,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.79,"TRtn1Q":null,"TRtn2":4.78,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.83,"PctSucVlvQ":null,"TSup1":3.96,"TSup1Q":null,"TSup2":3.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:15:28.155Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6d62729e-c960-4ab8-8c28-9104c53575cf","EventDtm":"2025-11-27T13:15:09Z","AppDtm":"2025-11-27T13:15:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:15:09Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804926,"GPSLongitude":77.662245,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:15:09Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":29.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":89,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.54,"AmpPhB":11.14,"AmpPhC":11.54,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.13,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.39,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.01,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.68,"TRtn1Q":null,"TRtn2":5.7,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.41,"PctSucVlvQ":null,"TSup1":4.99,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
   </si>
 </sst>
 </file>
@@ -492,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -799,70 +787,6 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Merge main branch into feature/technician-location-editing
- Merged latest changes from main including package updates and route improvements
- Resolved conflicts in log files by keeping local changes
- Branch now contains both feature changes and latest main updates
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-27.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="101">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,55 +43,277 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-27T13:07:24.620Z</t>
+    <t>2025-11-27T17:30:31.567Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d74318a2-e69a-4a80-85f2-2d89cb19662d","EventDtm":"2025-11-27T12:59:44Z","AppDtm":"2025-11-27T13:00:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T12:59:44Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.539016,"GPSLongitude":78.178353,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.4,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T12:59:44Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":26.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":112.6,"TDisQ":null,"FreqComp":null,"TSuc":-35.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:07:24.662Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"09f1e680-1dd7-4dac-9818-58bd20690ea0","EventDtm":"2025-11-27T13:01:29Z","AppDtm":"2025-11-27T13:01:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:01:29Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533149,"GPSLongitude":78.433604,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:01:29Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":25.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":71.8,"TDisQ":null,"FreqComp":null,"TSuc":-30.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":418.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6.2,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:07:24.670Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"35b4b8b4-29e0-407f-a66b-85af65516e97","EventDtm":"2025-11-27T13:02:23Z","AppDtm":"2025-11-27T13:02:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:02:23Z","DeviceID":"JSGA623040321","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.816183,"GPSLongitude":77.687294,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9057","CID":"180498700","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6617250","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:07:24.674Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1d989149-95b7-40d7-b424-e5d22bd41a94","EventDtm":"2025-11-27T13:04:53Z","AppDtm":"2025-11-27T13:05:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:04:53Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":26.644409,"GPSLongitude":88.467959,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8.1,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:04:53Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":23.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-50,"PSucQ":"asProvided","TDis":96.8,"TDisQ":null,"FreqComp":null,"TSuc":-29.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":790,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":12,"PctExpVlvQ":null,"TEvap":-0.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.81,"TRtn1Q":null,"TRtn2":1.6,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.76,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.7,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:07:24.679Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7df7cac5-50df-4a89-bf26-f8c3322a4554","EventDtm":"2025-11-27T13:05:03Z","AppDtm":"2025-11-27T13:05:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:05:03Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.80499,"GPSLongitude":77.662225,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:05:03Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":29.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":88.22,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.66,"AmpPhB":11.27,"AmpPhC":11.66,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.14,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.71,"TRtn1Q":null,"TRtn2":5.72,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.58,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:09:05.762Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c74ecaba-9185-482a-8953-b954c8f22456","EventDtm":"2025-11-27T13:08:48Z","AppDtm":"2025-11-27T13:09:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:08:48Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":16.824945,"GPSLongitude":78.131517,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:08:48Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":26.12,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":72.5,"TDisQ":null,"FreqComp":null,"TSuc":-26.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.81,"TRtn1Q":null,"TRtn2":4.6,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:10:42.027Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"14d7f88e-0174-46bf-b976-47340e246acd","EventDtm":"2025-11-27T13:10:18Z","AppDtm":"2025-11-27T13:10:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:10:18Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.661607,"GPSLongitude":83.089135,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.8,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:10:18Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":42.9,"TDisQ":null,"FreqComp":null,"TSuc":-15.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":970,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":373.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":92.68,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-27T13:11:26.371Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0917fa97-7d41-4329-a671-d94bb2b525b6","EventDtm":"2025-11-27T13:11:05Z","AppDtm":"2025-11-27T13:11:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T13:11:05Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.537024,"GPSLongitude":78.175741,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T13:11:05Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":26.59,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":153.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":10.05,"AmpPhB":11.44,"AmpPhC":10.05,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.58,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":8.31,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.36,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.81,"TRtn1Q":null,"TRtn2":-17.82,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.58,"TSup1Q":null,"TSup2":-31.8,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"78ea24c5-c925-4574-bb3d-86c154c4c43b","EventDtm":"2025-11-27T17:10:26Z","AppDtm":"2025-11-27T17:10:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:10:26Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661584,"GPSLongitude":83.089108,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:10:26Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":22.38,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":80,"PSucQ":"asProvided","TDis":40.9,"TDisQ":null,"FreqComp":null,"TSuc":30.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":31,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":388.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.19,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":87.8,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:31.929Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"91eaa231-7076-4565-987c-83a1a1f279e9","EventDtm":"2025-11-27T17:10:57Z","AppDtm":"2025-11-27T17:11:21Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:10:57Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.537028,"GPSLongitude":78.17574,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:10:57Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":24.09,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":146.45,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":10.69,"AmpPhB":12.18,"AmpPhC":10.69,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.93,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":17.96,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":423.69,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.97,"TRtn1Q":null,"TRtn2":-17.99,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-31.83,"TSup1Q":null,"TSup2":-30.85,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.156Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"22894f0e-fcf7-44b4-8970-bb1fea408f75","EventDtm":"2025-11-27T17:14:47Z","AppDtm":"2025-11-27T17:15:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:14:47Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.679061,"GPSLongitude":78.720199,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:14:47Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":23.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-181.25,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":175.23,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":9.49,"AmpPhB":10.29,"AmpPhC":9.49,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.17,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":407.37,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.08,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.67,"TRtn1Q":null,"TRtn2":4.67,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.61,"PctSucVlvQ":null,"TSup1":4.08,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.349Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e1a16d51-6c4a-40ea-bff5-af40b18fb435","EventDtm":"2025-11-27T17:15:08Z","AppDtm":"2025-11-27T17:15:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:15:08Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.804981,"GPSLongitude":77.662252,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:15:08Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.65,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":85.69,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.47,"AmpPhB":10.82,"AmpPhC":11.47,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.08,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.9,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.64,"TRtn1Q":null,"TRtn2":5.65,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.96,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.458Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5a373ded-6fda-438a-9f2d-b3e492504512","EventDtm":"2025-11-27T17:20:13Z","AppDtm":"2025-11-27T17:20:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:20:13Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":15.479462,"GPSLongitude":73.969679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:20:13Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":25.24,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":134.98,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.5,"AmpPhB":10.15,"AmpPhC":10.5,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.98,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.02,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.34,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.04,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.6,"TRtn1Q":null,"TRtn2":5.62,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.9,"PctSucVlvQ":null,"TSup1":5.05,"TSup1Q":null,"TSup2":5.06,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.501Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"efda0fae-9604-4517-aa57-e5b24571ff11","EventDtm":"2025-11-27T17:22:46Z","AppDtm":"2025-11-27T17:23:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:22:46Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.516025,"GPSLongitude":82.981153,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:22:46Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":24.31,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.48,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":167.39,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.12,"AmpPhB":10.94,"AmpPhC":11.12,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.11,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.59,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.53,"TRtn1Q":null,"TRtn2":3.58,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.17,"PctSucVlvQ":null,"TSup1":2.93,"TSup1Q":null,"TSup2":2.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.563Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"80445723-b3d6-4b94-bea2-749664297da4","EventDtm":"2025-11-27T17:23:10Z","AppDtm":"2025-11-27T17:23:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:23:10Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.533321,"GPSLongitude":78.43305,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.7,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:23:10Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":23.5,"TAmbQ":null,"TUSDA4":-46.2,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":44.4,"TDisQ":null,"FreqComp":null,"TSuc":5.6,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":760,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":18.11,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":426.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.38,"TRtn1Q":null,"TRtn2":136.6,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":79.57,"PctSucVlvQ":null,"TSup1":4.81,"TSup1Q":null,"TSup2":4.8,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.640Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f2bb89b7-f1d8-436d-b1d4-638d491d471a","EventDtm":"2025-11-27T17:25:13Z","AppDtm":"2025-11-27T17:25:31Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:25:13Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804934,"GPSLongitude":77.662245,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:25:13Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.63,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":82.08,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.37,"AmpPhB":11.01,"AmpPhC":11.37,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.11,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.62,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.02,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.66,"TRtn1Q":null,"TRtn2":5.68,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.47,"PctSucVlvQ":null,"TSup1":5.02,"TSup1Q":null,"TSup2":4.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.693Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8a6f2ab2-e4a1-4d1e-a0ff-27c5f396ad95","EventDtm":"2025-11-27T17:25:19Z","AppDtm":"2025-11-27T17:25:41Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:25:19Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":21.735542,"GPSLongitude":72.628797,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"236857089","RSSI":"-61","ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:25:19Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":28.87,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":153.08,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.69,"AmpPhB":13.41,"AmpPhC":13.69,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90.76,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":436.55,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.11,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.51,"TRtn1Q":null,"TRtn2":15.46,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.49,"PctSucVlvQ":null,"TSup1":15.16,"TSup1Q":null,"TSup2":15.33,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.726Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"85b90d74-5b9a-4a03-8845-49d9ac627b57","EventDtm":"2025-11-27T17:25:46Z","AppDtm":"2025-11-27T17:26:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:25:46Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.54775,"GPSLongitude":78.380563,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8.1,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:30:32.766Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"789a89d3-476b-4d43-bffd-79dd3a638c63","EventDtm":"2025-11-27T17:28:00Z","AppDtm":"2025-11-27T17:28:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:28:00Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.516249,"GPSLongitude":82.96235,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957963","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:28:00Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":22,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":30,"PSucQ":"asProvided","TDis":83.1,"TDisQ":null,"FreqComp":null,"TSuc":-13.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":84,"PctExpVlvQ":null,"TEvap":22.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":391.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.4,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.45,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:32:47.532Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"432d588b-5ace-47ef-ae74-d9f83b9f9200","EventDtm":"2025-11-27T17:32:35Z","AppDtm":"2025-11-27T17:32:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:32:35Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":19.252895,"GPSLongitude":73.016511,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:32:47.645Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"31e92aa7-3a56-4169-be61-189291daa4fa","EventDtm":"2025-11-27T17:32:33Z","AppDtm":"2025-11-27T17:32:46Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:32:33Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":28.364659,"GPSLongitude":75.581324,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"144900619","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":22,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:32:33Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":15,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":34,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":6.2,"AmpPhB":6.7,"AmpPhC":7.2,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":16.9,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":6.6,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:35:25.645Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e3f6c27f-b43e-4423-a543-6256a204a20d","EventDtm":"2025-11-27T17:35:09Z","AppDtm":"2025-11-27T17:35:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:35:09Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.804997,"GPSLongitude":77.662265,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:35:09Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.65,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":81.9,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.5,"AmpPhB":10.96,"AmpPhC":11.5,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.15,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.34,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.07,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.7,"TRtn1Q":null,"TRtn2":5.71,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.72,"PctSucVlvQ":null,"TSup1":5.07,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:36:23.382Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d11fe4e5-cf82-4610-8006-2fbf77a8452b","EventDtm":"2025-11-27T17:36:10Z","AppDtm":"2025-11-27T17:36:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:36:10Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.657847,"GPSLongitude":83.101826,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:36:10Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":24.55,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":68.51,"PSucQ":null,"TDis":-189.45,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":95.82,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.93,"AmpPhB":1.55,"AmpPhC":0.93,"PDis":95.89,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.55,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.02,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":422.15,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.29,"TRtn1Q":null,"TRtn2":20.35,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":21,"PctSucVlvQ":null,"TSup1":19.57,"TSup1Q":null,"TSup2":19.66,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:39:25.411Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4105d945-4475-4501-aada-decf1485220c","EventDtm":"2025-11-27T17:39:10Z","AppDtm":"2025-11-27T17:39:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:39:10Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.892013,"GPSLongitude":79.476318,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:39:10Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":23.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":77.6,"TDisQ":null,"FreqComp":null,"TSuc":-30.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":730,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":19,"PctExpVlvQ":null,"TEvap":-0.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.38,"TRtn1Q":null,"TRtn2":4.9,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:39:52.538Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"71913497-12cb-4540-a47f-79e2862b8f9a","EventDtm":"2025-11-27T17:39:33Z","AppDtm":"2025-11-27T17:39:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:39:33Z","DeviceID":"JSGA623040314","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":19.252922,"GPSLongitude":73.016541,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.3,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:39:33Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":18.95,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":115.33,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Defrost","SnCtrl":"04547502","AmpPhA":5.11,"AmpPhB":5.18,"AmpPhC":5.18,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":8.33,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":426.07,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.85,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.86,"TRtn1Q":null,"TRtn2":5.99,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":0,"PctSucVlvQ":null,"TSup1":9.09,"TSup1Q":null,"TSup2":5.84,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:44:01.206Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e73024d7-4b72-443b-9243-428319ca5593","EventDtm":"2025-11-27T17:43:46Z","AppDtm":"2025-11-27T17:44:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:43:46Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":9,"GPSLastLock":37,"GPSLatitude":17.548039,"GPSLongitude":78.380424,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-61","ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:44:01.792Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"85ac91eb-4bdb-470b-b252-95e7f4939fa2","EventDtm":"2025-11-27T17:43:42Z","AppDtm":"2025-11-27T17:44:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:43:42Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.657848,"GPSLongitude":83.101714,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"248666903","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":7.9,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:43:42Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":24.84,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":70.64,"PSucQ":null,"TDis":-191.41,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":92.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.94,"AmpPhB":1.58,"AmpPhC":0.94,"PDis":112.22,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.38,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.99,"TRtn1Q":null,"TRtn2":21.02,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":21,"PctSucVlvQ":null,"TSup1":21.13,"TSup1Q":null,"TSup2":21.15,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:44:42.001Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d74fbadf-d347-42cf-9c23-694e66092b18","EventDtm":"2025-11-27T17:44:26Z","AppDtm":"2025-11-27T17:44:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:44:26Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":12.804968,"GPSLongitude":77.662246,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.4,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:44:26Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":19.11,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":82.42,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":11.18,"AmpPhB":10.78,"AmpPhC":11.18,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.91,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.32,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.29,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.28,"TRtn1Q":null,"TRtn2":5.28,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.78,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.95,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:44:45.499Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"db4d7638-ab99-4e5a-a468-0b44c274b809","EventDtm":"2025-11-27T17:44:27Z","AppDtm":"2025-11-27T17:44:46Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:44:27Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":16.892038,"GPSLongitude":79.4763,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:44:27Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":24.26,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":171.63,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":10.33,"AmpPhB":10.15,"AmpPhC":10.33,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.22,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.2,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":403.03,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.95,"TRtn1Q":null,"TRtn2":17.9,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.11,"PctSucVlvQ":null,"TSup1":18.57,"TSup1Q":null,"TSup2":18.6,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:45:25.575Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3dc03c76-788b-486e-9ce9-9e1d8c9e5d3e","EventDtm":"2025-11-27T17:45:09Z","AppDtm":"2025-11-27T17:45:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:45:09Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.805066,"GPSLongitude":77.662171,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:45:09Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.15,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":82.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.89,"AmpPhB":11.18,"AmpPhC":11.89,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.09,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":420.03,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.66,"TRtn1Q":null,"TRtn2":5.67,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.65,"PctSucVlvQ":null,"TSup1":4.92,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:47:32.821Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"13bb352c-0798-4e1e-8400-7aba1163710b","EventDtm":"2025-11-27T17:46:54Z","AppDtm":"2025-11-27T17:47:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:46:54Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.572208,"GPSLongitude":78.515147,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323414","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":33.7,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:48:05.312Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":24,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4576e754-f623-490e-a7c5-e42fff5c4dd0","EventDtm":"2025-11-27T17:47:49Z","AppDtm":"2025-11-27T17:48:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:47:49Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":26.310525,"GPSLongitude":91.717546,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551307","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.2,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:47:49Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":19.81,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":70.1,"TDisQ":null,"FreqComp":null,"TSuc":-31.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":100,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":418.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":82.62,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:49:36.961Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":25,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"cb61341d-f3cb-4e31-ba26-7e2fe0b15d24","EventDtm":"2025-11-27T17:49:18Z","AppDtm":"2025-11-27T17:49:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:49:18Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.891744,"GPSLongitude":79.475855,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:49:18Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":23.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":67.3,"TDisQ":null,"FreqComp":null,"TSuc":-33.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":780,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":35,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":8.54,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:50:40.528Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":26,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8f94cf6e-88b5-4701-a160-0dff74af22ad","EventDtm":"2025-11-27T17:50:08Z","AppDtm":"2025-11-27T17:50:41Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:50:08Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":26.606148,"GPSLongitude":80.723717,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34.3,"BatteryVoltage":8,"DeviceTemp":17,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:55:26.236Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":27,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"062d4d6d-b54d-4e8a-b369-68d26973710b","EventDtm":"2025-11-27T17:55:10Z","AppDtm":"2025-11-27T17:55:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:55:10Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.80501,"GPSLongitude":77.662182,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:55:10Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":81.34,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.66,"AmpPhB":11.12,"AmpPhC":11.66,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.07,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":420.83,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.63,"TRtn1Q":null,"TRtn2":5.65,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.15,"PctSucVlvQ":null,"TSup1":4.98,"TSup1Q":null,"TSup2":4.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:55:37.312Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":28,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a618b0e6-95e1-4215-82d8-93dadf31fbe2","EventDtm":"2025-11-27T19:37:40Z","AppDtm":"2025-11-27T17:55:38Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T19:37:40Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":7346,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T17:58:24.638Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":29,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4c69cee7-1ca8-48f9-ac42-27bebfe81bd2","EventDtm":"2025-11-27T17:58:05Z","AppDtm":"2025-11-27T17:58:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T17:58:05Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":28.678646,"GPSLongitude":77.599851,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T17:58:05Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":18.18,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":61.37,"PSucQ":null,"TDis":48.27,"TDisQ":null,"FreqComp":null,"TSuc":17.25,"TSucQ":null,"MCond":0,"PCond":272.85,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04475864","AmpPhA":1.58,"AmpPhB":1.51,"AmpPhC":1.58,"PDis":93.04,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":17.44,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":64.79,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.47,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":16.99,"TRtn1Q":null,"TRtn2":16.99,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":20,"PctSucVlvQ":null,"TSup1":17.38,"TSup1Q":null,"TSup2":17.4,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:00:33.488Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":30,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"18617b6f-4152-4995-9fa9-632c3708e5c4","EventDtm":"2025-11-27T18:00:18Z","AppDtm":"2025-11-27T18:00:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:00:18Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.539015,"GPSLongitude":78.178211,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:00:18Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":22.5,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":78.1,"TDisQ":null,"FreqComp":null,"TSuc":-18.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":409.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.88,"TRtn1Q":null,"TRtn2":4.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":83.54,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:02:53.845Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":31,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1dd58032-b1cf-4087-818a-9ae721b33327","EventDtm":"2025-11-27T18:02:33Z","AppDtm":"2025-11-27T18:02:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:02:33Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.533057,"GPSLongitude":78.43347,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.2,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:02:33Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":22.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":79,"TDisQ":null,"FreqComp":null,"TSuc":-33.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":780,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":422.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.88,"TRtn1Q":null,"TRtn2":6,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.15,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.2,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:03:29.885Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":32,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"17499607-05b3-4fac-a8e9-5a654133d8d8","EventDtm":"2025-11-27T18:03:11Z","AppDtm":"2025-11-27T18:03:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:03:11Z","DeviceID":"JSGA623040321","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.816361,"GPSLongitude":77.687215,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9057","CID":"180498700","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":31.8,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6617250","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:05:27.034Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":33,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c4c816ba-d363-4175-b271-c23b23aa8bee","EventDtm":"2025-11-27T18:05:14Z","AppDtm":"2025-11-27T18:05:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:05:14Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":26.644522,"GPSLongitude":88.467979,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.4,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:05:14Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":20.19,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":76.5,"TDisQ":null,"FreqComp":null,"TSuc":-14.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":-0.69,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":421.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.69,"TRtn1Q":null,"TRtn2":1.4,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":18.29,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:05:28.067Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":34,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0c5995ac-2909-4b9f-8875-ecd7da99b644","EventDtm":"2025-11-27T18:05:12Z","AppDtm":"2025-11-27T18:05:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:05:12Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.804932,"GPSLongitude":77.662205,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:05:12Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.26,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":81,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.3,"AmpPhB":10.91,"AmpPhC":11.3,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.16,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.72,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.09,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.7,"TRtn1Q":null,"TRtn2":5.72,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.74,"PctSucVlvQ":null,"TSup1":5.09,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:09:50.765Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":35,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a54f9eb4-4fd2-41c4-8c5a-5ac9a6c1b8f0","EventDtm":"2025-11-27T18:09:33Z","AppDtm":"2025-11-27T18:09:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:09:33Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":16.824899,"GPSLongitude":78.131498,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:09:33Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":21.31,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":57.3,"TDisQ":null,"FreqComp":null,"TSuc":-28,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":10.19,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":400.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":4.5,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.45,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:10:50.035Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":36,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4d332336-7a45-47be-9677-bf7493070cff","EventDtm":"2025-11-27T18:10:29Z","AppDtm":"2025-11-27T18:10:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:10:29Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661569,"GPSLongitude":83.089132,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:10:29Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":21.81,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":20,"PSucQ":"asProvided","TDis":39.4,"TDisQ":null,"FreqComp":null,"TSuc":-20.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":870,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":387.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":86.89,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.7,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:11:20.029Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":37,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d3dba96f-d0c1-496f-b19f-58194a08092d","EventDtm":"2025-11-27T18:10:56Z","AppDtm":"2025-11-27T18:11:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:10:56Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.537125,"GPSLongitude":78.175612,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:10:56Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":24.16,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":179.23,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":10.73,"AmpPhB":12.21,"AmpPhC":10.73,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-24.04,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":14.66,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":425.12,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-18.1,"TRtn1Q":null,"TRtn2":-18.13,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.17,"TSup1Q":null,"TSup2":-31.32,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true},{"OemAlarm":72,"RCAlias":"AL72","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:15:17.528Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":38,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ef117706-515e-4dec-be69-cb04db516109","EventDtm":"2025-11-27T18:14:59Z","AppDtm":"2025-11-27T18:15:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:14:59Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.679083,"GPSLongitude":78.720202,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:14:59Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":22.54,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-178.91,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":167.15,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":9.58,"AmpPhB":10.45,"AmpPhC":9.58,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":406.28,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.11,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.62,"TRtn1Q":null,"TRtn2":4.62,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.91,"PctSucVlvQ":null,"TSup1":3.92,"TSup1Q":null,"TSup2":3.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:15:27.104Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":39,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fc6485f2-2c87-47ea-8733-3d4b7c781e07","EventDtm":"2025-11-27T18:15:11Z","AppDtm":"2025-11-27T18:15:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:15:11Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804918,"GPSLongitude":77.662202,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:15:11Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":83.18,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.47,"AmpPhB":11.01,"AmpPhC":11.47,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.62,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.66,"TRtn1Q":null,"TRtn2":5.68,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.54,"PctSucVlvQ":null,"TSup1":4.95,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:20:26.785Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":40,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"32078c8e-ec50-4121-a115-5c5174b46ca9","EventDtm":"2025-11-27T18:20:11Z","AppDtm":"2025-11-27T18:20:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:20:11Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":15.479435,"GPSLongitude":73.969672,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:20:11Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":24.39,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":131.31,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.36,"AmpPhB":10.01,"AmpPhC":10.36,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.92,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.44,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.04,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.54,"TRtn1Q":null,"TRtn2":5.56,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.57,"PctSucVlvQ":null,"TSup1":4.99,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:23:00.171Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":41,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e4ac9b5a-56f4-4d2b-a29d-241a8210ba63","EventDtm":"2025-11-27T18:22:42Z","AppDtm":"2025-11-27T18:23:01Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:22:42Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.516027,"GPSLongitude":82.981186,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:22:42Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":23.08,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.48,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":106.58,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":12,"AmpPhB":11.12,"AmpPhC":12,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.04,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.1,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.12,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.5,"TRtn1Q":null,"TRtn2":3.54,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.06,"PctSucVlvQ":null,"TSup1":2.92,"TSup1Q":null,"TSup2":2.97,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:23:29.248Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":42,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"81cda5ee-378b-42f0-a0a5-716bb5041741","EventDtm":"2025-11-27T18:23:13Z","AppDtm":"2025-11-27T18:23:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:23:13Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.533246,"GPSLongitude":78.433087,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:23:13Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":23.38,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":43.5,"TDisQ":null,"FreqComp":null,"TSuc":5.8,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":740,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":16.93,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":429.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.38,"TRtn1Q":null,"TRtn2":136.1,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":78.66,"PctSucVlvQ":null,"TSup1":4.81,"TSup1Q":null,"TSup2":4.9,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.2,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:25:27.544Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":43,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5657e823-cd49-492c-983e-d4c806bef430","EventDtm":"2025-11-27T18:25:11Z","AppDtm":"2025-11-27T18:25:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:25:11Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804919,"GPSLongitude":77.662199,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:25:11Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.72,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":86.86,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.44,"AmpPhB":11,"AmpPhC":11.44,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.08,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.96,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.63,"TRtn1Q":null,"TRtn2":5.65,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.53,"PctSucVlvQ":null,"TSup1":5.03,"TSup1Q":null,"TSup2":4.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:25:32.779Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":44,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ca812b0a-2d52-45ce-ad08-b070c254a1b3","EventDtm":"2025-11-27T18:25:15Z","AppDtm":"2025-11-27T18:25:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:25:15Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":21.735733,"GPSLongitude":72.628707,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.1,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-27T18:25:15Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":28.51,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":152.15,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.68,"AmpPhB":13.42,"AmpPhC":13.68,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.23,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":91.16,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":432.36,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.09,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.52,"TRtn1Q":null,"TRtn2":15.47,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.45,"PctSucVlvQ":null,"TSup1":15.1,"TSup1Q":null,"TSup2":15.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-27T18:26:08.510Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":45,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"83f8b65a-820b-4ee6-a4a1-ae38fb68a18f","EventDtm":"2025-11-27T18:25:51Z","AppDtm":"2025-11-27T18:26:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-27T18:25:51Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.547771,"GPSLongitude":78.380584,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":22,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
   </si>
 </sst>
 </file>
@@ -480,7 +702,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -787,6 +1009,1190 @@
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" t="s">
+        <v>11</v>
+      </c>
+      <c r="J45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>11</v>
+      </c>
+      <c r="J46" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>